<commit_message>
Correction de note sprint1
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3b2\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{623BACF4-43CD-438F-A885-B9773F8658D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7777432-A26B-48C3-B4A9-9F8B79BF2D21}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{623BACF4-43CD-438F-A885-B9773F8658D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{76184BF5-5D1B-497E-AEEA-03699F7A3C7F}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Sudoku" sheetId="1" state="hidden" r:id="rId1"/>
@@ -386,7 +386,7 @@
     <t>Point d'entrée dans l'application</t>
   </si>
   <si>
-    <t>Votre guide utilisateur aurait du être une page HTML, mais au moins vous avez créé du contenu alors pas mal..Pas de tests......</t>
+    <t>Votre guide utilisateur aurait du être une page HTML, mais au moins vous avez créé du contenu alors pas mal..Pas de tests......| Recorrection: Les tests sont bien là, mais ils sont aussi dans le Sidebar component</t>
   </si>
   <si>
     <t>ER</t>
@@ -395,13 +395,13 @@
     <t>Vue de dessin</t>
   </si>
   <si>
-    <t>Impossible de créer un dessin...</t>
+    <t>Impossible de créer un dessin...|Recorrection: Barre défilement verticale non présente, mais scrollable</t>
   </si>
   <si>
     <t>Créer un nouveau dessin</t>
   </si>
   <si>
-    <t>Le raccourci ouvre deux fenêtres: votre modale et l'action du browser (il vous manque preventDefault). Le redimensionnement ne change pas les valeurs des dimensions dans le form, je pense que vous avez implémenté la mauvaise chose.. La validation ne devrait pas nécessairement tout enlever les valeurs . Le formulaire ne crée pas de dessin sur ma version.. Sinon le reste semble plus ou moin bon.</t>
+    <t>Le raccourci ouvre deux fenêtres: votre modale et l'action du browser (il vous manque preventDefault). Le redimensionnement ne change pas les valeurs des dimensions dans le form, je pense que vous avez implémenté la mauvaise chose.. La validation ne devrait pas nécessairement tout enlever les valeurs . Le formulaire ne crée pas de dessin sur ma version.. Sinon le reste semble plus ou moin bon.|Recorrection: Fonctionnalités: pour le redimensionnement OK.</t>
   </si>
   <si>
     <t>Outil de couleur</t>
@@ -6359,15 +6359,15 @@
       </c>
       <c r="B4" s="275">
         <f>(Fonctionnalité!E16)</f>
-        <v>0.62350000000000005</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="C4" s="190">
         <f>'Assurance Qualité'!B49</f>
-        <v>0.83499999999999996</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="D4" s="190">
         <f>AVERAGE(B4:C4) - 0.1*E4</f>
-        <v>0.72924999999999995</v>
+        <v>0.88375000000000004</v>
       </c>
       <c r="G4" s="276">
         <v>1</v>
@@ -6443,8 +6443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6628,14 +6628,14 @@
         <v>1</v>
       </c>
       <c r="C9" s="231">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="231">
         <v>15</v>
       </c>
       <c r="E9" s="231">
         <f t="shared" ref="E9:E15" si="0">B9*C9*D9</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F9" s="232" t="s">
         <v>114</v>
@@ -6657,7 +6657,7 @@
         <v>116</v>
       </c>
       <c r="B10" s="231">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C10" s="231">
         <v>1</v>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="E10" s="231">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.399999999999999</v>
       </c>
       <c r="F10" s="232" t="s">
         <v>117</v>
@@ -6684,12 +6684,12 @@
       <c r="N10" s="223"/>
       <c r="O10" s="223"/>
     </row>
-    <row r="11" spans="1:15" ht="120">
+    <row r="11" spans="1:15" ht="150">
       <c r="A11" s="230" t="s">
         <v>118</v>
       </c>
       <c r="B11" s="231">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="C11" s="231">
         <v>1</v>
@@ -6699,7 +6699,7 @@
       </c>
       <c r="E11" s="231">
         <f t="shared" si="0"/>
-        <v>11.25</v>
+        <v>12.75</v>
       </c>
       <c r="F11" s="209" t="s">
         <v>119</v>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="E16" s="277">
         <f>SUM(E8:E15)/D16 - E18*D18 - E17*D17</f>
-        <v>0.62350000000000005</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="F16" s="236"/>
     </row>
@@ -7504,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C68761-F424-44AF-8353-006282F54B4A}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -7666,7 +7666,7 @@
         <v>160</v>
       </c>
       <c r="B9" s="208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="209">
         <v>3</v>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="B10" s="211">
         <f>SUMPRODUCT(B8:B9,C8:C9)</f>
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="C10" s="212">
         <f>SUM(C8:C9)</f>
@@ -8604,7 +8604,7 @@
       </c>
       <c r="B48" s="218">
         <f>B10+B15+B20+B25+B30+B41+B46</f>
-        <v>83.5</v>
+        <v>86.5</v>
       </c>
       <c r="C48" s="219">
         <f>C10+C15+C20+C25+C30+C41+C46</f>
@@ -8641,7 +8641,7 @@
       </c>
       <c r="B49" s="318">
         <f>B48/C48</f>
-        <v>0.83499999999999996</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="C49" s="319"/>
       <c r="D49" s="320">

</xml_diff>

<commit_message>
Remise des notes du sprtin2
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3b2\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2ea9\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{623BACF4-43CD-438F-A885-B9773F8658D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{76184BF5-5D1B-497E-AEEA-03699F7A3C7F}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="13_ncr:1_{623BACF4-43CD-438F-A885-B9773F8658D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC74D888-DD65-4EB4-9A61-DFFB1D38FF94}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Sudoku" sheetId="1" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="216">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>Bonne analyse, mais vous auriez du ignorer les commits par rapport au cadriciel: ça fausse tout vos résultats et ça rend votre analyse incorrecte et moins fiable (gros problème). Si vous avez parlé de ça dans votre analyse, vous auriez pu re-faire vos graphiques. Attention au français. Comment est-ce que vous avez fait pour générer les graphiques 1 à 4 ?</t>
+  </si>
+  <si>
+    <t>Tous les elements demandés sont là. Bonne justification</t>
   </si>
   <si>
     <t>Grille de correction Projet 2</t>
@@ -418,8 +421,8 @@
     <t>Outil-Crayon</t>
   </si>
   <si>
-    <t>Le tracé sur firefox ne fonctionne pas tout le temps très bien
-Faire juste un clic ne fait pas exactement un point (visible avec un petit épaisseur</t>
+    <t xml:space="preserve">Le tracé sur firefox ne fonctionne pas tout le temps très bien
+</t>
   </si>
   <si>
     <t>Outil-Application de couleur</t>
@@ -437,36 +440,72 @@
     <t>Ne build pas</t>
   </si>
   <si>
+    <t>c7dd6e2ae4d916bf0e3953e15e8b3ea132446334</t>
+  </si>
+  <si>
     <t>Ouvrir un dessin-Serveur</t>
   </si>
   <si>
+    <t>Raccourci non fonctionnel. La liste doit être chargeable sans présenter trop de choix à l'utilisateur (max de 8 en même temps). Ne prends pas en compte la taille du dessin. Tests laissent a desirer</t>
+  </si>
+  <si>
     <t>Etiquettes</t>
   </si>
   <si>
+    <t>Pas de tag vide dans loading. FIltrage non fonctionnel parfois. Pas de test serveur. Tests laissent a desirer</t>
+  </si>
+  <si>
     <t>Sauvegarder le dessin-serveur</t>
   </si>
   <si>
+    <t>Raccourci non fonctionnel. La modale de sauvegarde (ou du moins le bouton de confirmation) est mise non disponbile lorsque le dessin est en pleine sauvegarde.  Des fois ca plante. Pas de test serveur adequat. Tests clients laissent a desirer</t>
+  </si>
+  <si>
     <t>Outil-Sélection et inversion de sélection</t>
   </si>
   <si>
+    <t>Selection non fonctionnelle sur Firefox. Pas d'inversion de selection sur la plupart des forms. Tests non adequats</t>
+  </si>
+  <si>
     <t>Grille(surface de dessin)</t>
   </si>
   <si>
+    <t xml:space="preserve">Le raccourci ne fonctionne pas
+Il devrait y avoir un seul bouton de type toggle
+La grille passe par dessus les traits
+</t>
+  </si>
+  <si>
     <t>Outil - Ligne</t>
   </si>
   <si>
+    <t>Mettez une valeur par défaut pour les radio buttons
+Appuyez sur shift arrête le trait. Pas possible de fermer une ligne avec shift + double clic
+Les jonctions par point ne fonctionnent pas sur Firefox</t>
+  </si>
+  <si>
     <t>Outil-Ellipse</t>
   </si>
   <si>
+    <t>Lorsqu'on a de la transparence, on se retrouve avec 2 bordures visibles</t>
+  </si>
+  <si>
     <t>Outil - Polygone</t>
   </si>
   <si>
+    <t>Lorsqu'on a de la transparence, on se retrouve avec 2 bordures visibles
+Vos polygones ne sont pas réguliers</t>
+  </si>
+  <si>
     <t>Outil- Pipette</t>
   </si>
   <si>
     <t>Outil-Étampe</t>
   </si>
   <si>
+    <t>Réglez les problèmes pour l'outil de couleur mentionné à la correction du sprint 1 pour le prochain sprint. Bonus 1% pipette</t>
+  </si>
+  <si>
     <t>Anciennes fonctionnalités brisées</t>
   </si>
   <si>
@@ -527,28 +566,43 @@
     <t>ShapesService a beaucoup trop de responsabilités.</t>
   </si>
   <si>
+    <t>Suggestion: pour votre backend, ne faites pas de database controller. Allez à un plus haut niveau.</t>
+  </si>
+  <si>
     <t>La classe minimise l'accessibilité des membres</t>
   </si>
   <si>
+    <t>FileParametersServiceService entre autres, ne minimise pas l'accès à ses membres</t>
+  </si>
+  <si>
+    <t>EllipseService entre autres ne minimise pas l'accès à ses attributs</t>
+  </si>
+  <si>
     <t>Total de la catégorie</t>
   </si>
   <si>
-    <t>FileParametersServiceService entre autres, ne minimise pas l'accès à ses membres</t>
-  </si>
-  <si>
     <t>Qualité des fonctions (Anes)</t>
   </si>
   <si>
     <t>La fonction ne fait qu'une chose et elle est non triviale. Son nom est clair, pertinent, représentatif de sa tâche et respecte les conventions.</t>
   </si>
   <si>
+    <t>SideBarComponent.selectTool ou onKeyDown ne snt pas DRY. Pensez à utiliser une map.</t>
+  </si>
+  <si>
     <t>L'ordre des paramètres est cohérent. (x, y, z) plutôt que (y, z, x) par exemple.</t>
   </si>
   <si>
     <t>Tous les paramètres de fonction sont utilisés</t>
   </si>
   <si>
-    <t>Exceptions (Anes)</t>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>Anes</t>
+  </si>
+  <si>
+    <t>Ryan</t>
   </si>
   <si>
     <t>Les constructeurs ne lancent pas d'exceptions</t>
@@ -560,7 +614,7 @@
     <t>Il n'y a pas de bloc "catch" vide, ou s'ils sont présents, ils sont documentés.</t>
   </si>
   <si>
-    <t>Variables (Anes)</t>
+    <t>Variables</t>
   </si>
   <si>
     <t>Les variables ont une seule raison-d'être (pas utilisées pour deux choses différentes)</t>
@@ -579,12 +633,15 @@
 Beaucoup de getter/setter inutiles.</t>
   </si>
   <si>
-    <t>Expression Booléennes (Anes)</t>
+    <t>Expression Booléennes</t>
   </si>
   <si>
     <t>Les expression booléennes ne sont pas comparées à true et false</t>
   </si>
   <si>
+    <t xml:space="preserve">line.service.ts. </t>
+  </si>
+  <si>
     <t>Utilisation des opérateurs ternaires dans les bon scénarii</t>
   </si>
   <si>
@@ -634,6 +691,9 @@
   </si>
   <si>
     <t>Le repo git ne contient que les fichiers nécessaires. (pas de dossier node_modules ou de package-lock.json et pas de package.json dans des dossiers autre que client ou server)</t>
+  </si>
+  <si>
+    <t>Présence de package-lock.json inutile à la racine du repo</t>
   </si>
   <si>
     <t xml:space="preserve">Total </t>
@@ -646,6 +706,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -2239,7 +2302,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="337">
+  <cellXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2912,22 +2975,31 @@
     <xf numFmtId="10" fontId="12" fillId="19" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3005,6 +3077,36 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="12" borderId="79" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3017,15 +3119,6 @@
     <xf numFmtId="9" fontId="0" fillId="13" borderId="77" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="17" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3038,10 +3131,10 @@
     <xf numFmtId="9" fontId="0" fillId="17" borderId="77" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="79" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="77" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="79" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="77" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3054,27 +3147,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="16" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3883,18 +3955,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:11" ht="15">
-      <c r="C2" s="284" t="s">
+      <c r="C2" s="287" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="284"/>
-      <c r="E2" s="285" t="s">
+      <c r="D2" s="287"/>
+      <c r="E2" s="288" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="285"/>
-      <c r="G2" s="286" t="s">
+      <c r="F2" s="288"/>
+      <c r="G2" s="289" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="286"/>
+      <c r="H2" s="289"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="138"/>
@@ -4175,7 +4247,7 @@
       <c r="F2" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="287" t="s">
+      <c r="G2" s="290" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4188,7 +4260,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="29"/>
       <c r="F3" s="33"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="291"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickTop="1">
       <c r="A4" s="76" t="s">
@@ -4505,21 +4577,21 @@
       <c r="A27" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="289" t="s">
+      <c r="H27" s="292" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="290"/>
+      <c r="I27" s="293"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1">
       <c r="A28" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="333" t="s">
+      <c r="B28" s="336" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="334"/>
-      <c r="D28" s="335"/>
-      <c r="E28" s="336"/>
+      <c r="C28" s="337"/>
+      <c r="D28" s="338"/>
+      <c r="E28" s="339"/>
       <c r="F28" s="94"/>
       <c r="H28" s="4" t="s">
         <v>58</v>
@@ -4856,7 +4928,7 @@
       <c r="F2" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="287" t="s">
+      <c r="G2" s="290" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4869,7 +4941,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="29"/>
       <c r="F3" s="33"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="291"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickTop="1">
       <c r="A4" s="76" t="s">
@@ -5238,21 +5310,21 @@
       <c r="A31" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="289" t="s">
+      <c r="H31" s="292" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="290"/>
+      <c r="I31" s="293"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1">
       <c r="A32" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="333" t="s">
+      <c r="B32" s="336" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="334"/>
-      <c r="D32" s="335"/>
-      <c r="E32" s="336"/>
+      <c r="C32" s="337"/>
+      <c r="D32" s="338"/>
+      <c r="E32" s="339"/>
       <c r="F32" s="94"/>
       <c r="H32" s="4" t="s">
         <v>58</v>
@@ -5589,7 +5661,7 @@
       <c r="F2" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="287" t="s">
+      <c r="G2" s="290" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5602,7 +5674,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="29"/>
       <c r="F3" s="33"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="291"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickTop="1">
       <c r="A4" s="76" t="s">
@@ -5997,21 +6069,21 @@
       <c r="A33" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="289" t="s">
+      <c r="H33" s="292" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="290"/>
+      <c r="I33" s="293"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1">
       <c r="A34" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="333" t="s">
+      <c r="B34" s="336" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="334"/>
-      <c r="D34" s="335"/>
-      <c r="E34" s="336"/>
+      <c r="C34" s="337"/>
+      <c r="D34" s="338"/>
+      <c r="E34" s="339"/>
       <c r="F34" s="94"/>
       <c r="H34" s="4" t="s">
         <v>58</v>
@@ -6316,7 +6388,7 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6327,13 +6399,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="279"/>
-      <c r="B2" s="279"/>
-      <c r="C2" s="279"/>
-      <c r="D2" s="279"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="279"/>
+      <c r="A3" s="285"/>
       <c r="B3" s="188" t="s">
         <v>98</v>
       </c>
@@ -6359,15 +6431,15 @@
       </c>
       <c r="B4" s="275">
         <f>(Fonctionnalité!E16)</f>
-        <v>0.90249999999999997</v>
+        <v>0.91449999999999998</v>
       </c>
       <c r="C4" s="190">
         <f>'Assurance Qualité'!B49</f>
-        <v>0.86499999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="D4" s="190">
         <f>AVERAGE(B4:C4) - 0.1*E4</f>
-        <v>0.88375000000000004</v>
+        <v>0.88224999999999998</v>
       </c>
       <c r="G4" s="276">
         <v>1</v>
@@ -6382,17 +6454,22 @@
       </c>
       <c r="B5" s="192">
         <f>(Fonctionnalité!E32)</f>
-        <v>0</v>
+        <v>0.65237500000000015</v>
       </c>
       <c r="C5" s="193">
         <f>'Assurance Qualité'!D49</f>
-        <v>0</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="D5" s="193">
         <f>AVERAGE(B5:C5) - 0.1*E5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="276"/>
+        <v>0.77368750000000008</v>
+      </c>
+      <c r="G5" s="276">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="194" t="s">
@@ -6443,8 +6520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6454,14 +6531,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A1" s="294" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
+      <c r="A1" s="297" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="298"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="298"/>
+      <c r="E1" s="298"/>
+      <c r="F1" s="298"/>
       <c r="G1" s="222"/>
       <c r="H1" s="222"/>
       <c r="I1" s="222"/>
@@ -6473,11 +6550,11 @@
       <c r="O1" s="223"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A2" s="279"/>
-      <c r="B2" s="279"/>
+      <c r="A2" s="285"/>
+      <c r="B2" s="285"/>
       <c r="C2" s="139"/>
       <c r="D2" s="139"/>
-      <c r="E2" s="279"/>
+      <c r="E2" s="285"/>
       <c r="F2" s="139"/>
       <c r="G2" s="224"/>
       <c r="H2" s="225"/>
@@ -6490,14 +6567,14 @@
       <c r="O2" s="223"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="297" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="295"/>
-      <c r="C3" s="295"/>
-      <c r="D3" s="295"/>
-      <c r="E3" s="295"/>
-      <c r="F3" s="295"/>
+      <c r="B3" s="298"/>
+      <c r="C3" s="298"/>
+      <c r="D3" s="298"/>
+      <c r="E3" s="298"/>
+      <c r="F3" s="298"/>
       <c r="G3" s="222"/>
       <c r="H3" s="222"/>
       <c r="I3" s="222"/>
@@ -6520,14 +6597,14 @@
       <c r="O4" s="223"/>
     </row>
     <row r="5" spans="1:15" ht="24" thickBot="1">
-      <c r="A5" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="296"/>
-      <c r="C5" s="296"/>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
+      <c r="A5" s="299" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="299"/>
+      <c r="C5" s="299"/>
+      <c r="D5" s="299"/>
+      <c r="E5" s="299"/>
+      <c r="F5" s="299"/>
       <c r="G5" s="223"/>
       <c r="H5" s="223"/>
       <c r="I5" s="223"/>
@@ -6542,13 +6619,13 @@
       <c r="A6" s="226" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="297" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="297"/>
-      <c r="D6" s="297"/>
-      <c r="E6" s="297"/>
-      <c r="F6" s="298"/>
+      <c r="B6" s="300" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="300"/>
+      <c r="D6" s="300"/>
+      <c r="E6" s="300"/>
+      <c r="F6" s="301"/>
       <c r="G6" s="227"/>
       <c r="H6" s="223"/>
       <c r="I6" s="223"/>
@@ -6561,19 +6638,19 @@
     </row>
     <row r="7" spans="1:15" ht="15">
       <c r="A7" s="206" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="228" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="228" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D7" s="228" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="228" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F7" s="229" t="s">
         <v>103</v>
@@ -6590,7 +6667,7 @@
     </row>
     <row r="8" spans="1:15" ht="25.15" customHeight="1">
       <c r="A8" s="230" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B8" s="231">
         <v>0.9</v>
@@ -6606,10 +6683,10 @@
         <v>10.8</v>
       </c>
       <c r="F8" s="209" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G8" s="227" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H8" s="223"/>
       <c r="I8" s="223"/>
@@ -6622,7 +6699,7 @@
     </row>
     <row r="9" spans="1:15" ht="15">
       <c r="A9" s="230" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" s="231">
         <v>1</v>
@@ -6638,10 +6715,10 @@
         <v>15</v>
       </c>
       <c r="F9" s="232" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G9" s="227" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H9" s="223"/>
       <c r="I9" s="223"/>
@@ -6654,7 +6731,7 @@
     </row>
     <row r="10" spans="1:15" ht="15">
       <c r="A10" s="230" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B10" s="231">
         <v>0.95</v>
@@ -6670,10 +6747,10 @@
         <v>11.399999999999999</v>
       </c>
       <c r="F10" s="232" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G10" s="227" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H10" s="223"/>
       <c r="I10" s="223"/>
@@ -6686,7 +6763,7 @@
     </row>
     <row r="11" spans="1:15" ht="150">
       <c r="A11" s="230" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B11" s="231">
         <v>0.85</v>
@@ -6702,10 +6779,10 @@
         <v>12.75</v>
       </c>
       <c r="F11" s="209" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G11" s="227" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H11" s="223"/>
       <c r="I11" s="223"/>
@@ -6718,7 +6795,7 @@
     </row>
     <row r="12" spans="1:15" ht="105">
       <c r="A12" s="230" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B12" s="231">
         <v>0.85</v>
@@ -6734,10 +6811,10 @@
         <v>10.199999999999999</v>
       </c>
       <c r="F12" s="209" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G12" s="227" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H12" s="223"/>
       <c r="I12" s="223"/>
@@ -6750,7 +6827,7 @@
     </row>
     <row r="13" spans="1:15" ht="18.75" customHeight="1">
       <c r="A13" s="230" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="231">
         <v>1</v>
@@ -6767,7 +6844,7 @@
       </c>
       <c r="F13" s="209"/>
       <c r="G13" s="227" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H13" s="223"/>
       <c r="I13" s="223"/>
@@ -6778,12 +6855,12 @@
       <c r="N13" s="223"/>
       <c r="O13" s="223"/>
     </row>
-    <row r="14" spans="1:15" ht="60">
+    <row r="14" spans="1:15" ht="45">
       <c r="A14" s="230" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B14" s="231">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C14" s="231">
         <v>1</v>
@@ -6793,13 +6870,13 @@
       </c>
       <c r="E14" s="231">
         <f t="shared" si="0"/>
-        <v>9.6000000000000014</v>
+        <v>10.8</v>
       </c>
       <c r="F14" s="209" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G14" s="233" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" s="234"/>
       <c r="I14" s="234"/>
@@ -6812,7 +6889,7 @@
     </row>
     <row r="15" spans="1:15" ht="15">
       <c r="A15" s="230" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B15" s="231">
         <v>0.85</v>
@@ -6828,237 +6905,325 @@
         <v>8.5</v>
       </c>
       <c r="F15" s="232" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="235" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="299"/>
-      <c r="C16" s="299"/>
-      <c r="D16" s="278">
+        <v>128</v>
+      </c>
+      <c r="B16" s="302"/>
+      <c r="C16" s="302"/>
+      <c r="D16" s="280">
         <f>SUM(D8:D15)</f>
         <v>100</v>
       </c>
       <c r="E16" s="277">
         <f>SUM(E8:E15)/D16 - E18*D18 - E17*D17</f>
-        <v>0.90249999999999997</v>
+        <v>0.91449999999999998</v>
       </c>
       <c r="F16" s="236"/>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="258" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D17" s="262">
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1">
       <c r="A18" s="258" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D18" s="262">
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="24" thickBot="1">
-      <c r="A19" s="305" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="306"/>
-      <c r="C19" s="306"/>
-      <c r="D19" s="306"/>
-      <c r="E19" s="306"/>
-      <c r="F19" s="306"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="24" thickBot="1">
+      <c r="A19" s="308" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="309"/>
+      <c r="C19" s="309"/>
+      <c r="D19" s="309"/>
+      <c r="E19" s="309"/>
+      <c r="F19" s="309"/>
+    </row>
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="307"/>
-      <c r="C20" s="308"/>
-      <c r="D20" s="308"/>
-      <c r="E20" s="308"/>
-      <c r="F20" s="308"/>
-    </row>
-    <row r="21" spans="1:6" ht="30.75" thickBot="1">
+      <c r="B20" s="310" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="311"/>
+      <c r="D20" s="311"/>
+      <c r="E20" s="311"/>
+      <c r="F20" s="311"/>
+    </row>
+    <row r="21" spans="1:7" ht="30.75" thickBot="1">
       <c r="A21" s="167" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B21" s="167" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="167" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D21" s="167" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="167" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F21" s="167" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+    <row r="22" spans="1:7" ht="60">
       <c r="A22" s="167" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="167"/>
-      <c r="C22" s="167"/>
+        <v>132</v>
+      </c>
+      <c r="B22" s="167">
+        <v>0.75</v>
+      </c>
+      <c r="C22" s="167">
+        <v>0.75</v>
+      </c>
       <c r="D22" s="167">
         <v>15</v>
       </c>
       <c r="E22" s="167">
         <f>B22*C22*D22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="167"/>
-    </row>
-    <row r="23" spans="1:6" ht="15">
+        <v>8.4375</v>
+      </c>
+      <c r="F22" s="167" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="167" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
+        <v>134</v>
+      </c>
+      <c r="B23" s="167">
+        <v>0.8</v>
+      </c>
+      <c r="C23" s="167">
+        <v>0.75</v>
+      </c>
       <c r="D23" s="167">
         <v>10</v>
       </c>
       <c r="E23" s="167">
         <f t="shared" ref="E23:E31" si="1">B23*C23*D23</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="167"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+        <v>6.0000000000000009</v>
+      </c>
+      <c r="F23" s="167" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75">
       <c r="A24" s="167" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="167"/>
-      <c r="C24" s="167"/>
+        <v>136</v>
+      </c>
+      <c r="B24" s="167">
+        <v>0.6</v>
+      </c>
+      <c r="C24" s="167">
+        <v>0.5</v>
+      </c>
       <c r="D24" s="167">
         <v>15</v>
       </c>
       <c r="E24" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="167"/>
-    </row>
-    <row r="25" spans="1:6" ht="15">
+        <v>4.5</v>
+      </c>
+      <c r="F24" s="167" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45">
       <c r="A25" s="167" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
+        <v>138</v>
+      </c>
+      <c r="B25" s="167">
+        <v>0.6</v>
+      </c>
+      <c r="C25" s="167">
+        <v>0.5</v>
+      </c>
       <c r="D25" s="167">
         <v>10</v>
       </c>
       <c r="E25" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="167"/>
-    </row>
-    <row r="26" spans="1:6" ht="15">
+        <v>3</v>
+      </c>
+      <c r="F25" s="167" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60">
       <c r="A26" s="167" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="167"/>
-      <c r="C26" s="167"/>
+        <v>140</v>
+      </c>
+      <c r="B26" s="167">
+        <v>0.75</v>
+      </c>
+      <c r="C26" s="167">
+        <v>1</v>
+      </c>
       <c r="D26" s="167">
         <v>10</v>
       </c>
       <c r="E26" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="167"/>
-    </row>
-    <row r="27" spans="1:6" ht="15">
+        <v>7.5</v>
+      </c>
+      <c r="F26" s="167" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60">
       <c r="A27" s="167" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="167"/>
-      <c r="C27" s="167"/>
+        <v>142</v>
+      </c>
+      <c r="B27" s="167">
+        <v>0.7</v>
+      </c>
+      <c r="C27" s="167">
+        <v>1</v>
+      </c>
       <c r="D27" s="167">
         <v>8</v>
       </c>
       <c r="E27" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="167"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+        <v>5.6</v>
+      </c>
+      <c r="F27" s="167" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="167" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
+        <v>144</v>
+      </c>
+      <c r="B28" s="167">
+        <v>0.9</v>
+      </c>
+      <c r="C28" s="167">
+        <v>1</v>
+      </c>
       <c r="D28" s="167">
         <v>8</v>
       </c>
       <c r="E28" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="167"/>
-    </row>
-    <row r="29" spans="1:6" ht="15">
+        <v>7.2</v>
+      </c>
+      <c r="F28" s="167" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45">
       <c r="A29" s="167" t="s">
-        <v>137</v>
-      </c>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
+        <v>146</v>
+      </c>
+      <c r="B29" s="167">
+        <v>0.75</v>
+      </c>
+      <c r="C29" s="167">
+        <v>1</v>
+      </c>
       <c r="D29" s="167">
         <v>8</v>
       </c>
       <c r="E29" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="167"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1">
+        <v>6</v>
+      </c>
+      <c r="F29" s="167" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" s="167" t="s">
-        <v>138</v>
-      </c>
-      <c r="B30" s="167"/>
-      <c r="C30" s="167"/>
+        <v>148</v>
+      </c>
+      <c r="B30" s="167">
+        <v>1</v>
+      </c>
+      <c r="C30" s="167">
+        <v>1</v>
+      </c>
       <c r="D30" s="167">
         <v>8</v>
       </c>
       <c r="E30" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F30" s="167"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1">
+      <c r="G30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15">
       <c r="A31" s="167" t="s">
-        <v>139</v>
-      </c>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
+        <v>149</v>
+      </c>
+      <c r="B31" s="167">
+        <v>1</v>
+      </c>
+      <c r="C31" s="167">
+        <v>1</v>
+      </c>
       <c r="D31" s="167">
         <v>8</v>
       </c>
       <c r="E31" s="167">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F31" s="167"/>
-    </row>
-    <row r="32" spans="1:6" ht="15">
+      <c r="G31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45">
       <c r="A32" s="243" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B32" s="243"/>
       <c r="C32" s="243"/>
@@ -7067,14 +7232,16 @@
         <v>100</v>
       </c>
       <c r="E32" s="255">
-        <f>SUM(E22:E30)/D32 -E33*D33 -E34*D34-E35*D35</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="243"/>
+        <f>SUM(E22:E31)/D32 -E33*D33 -E34*D34-E35*D35+1/100</f>
+        <v>0.65237500000000015</v>
+      </c>
+      <c r="F32" s="243" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15">
       <c r="A33" s="259" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D33" s="260">
         <v>0.15</v>
@@ -7082,7 +7249,7 @@
     </row>
     <row r="34" spans="1:6" ht="15">
       <c r="A34" s="259" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D34" s="261">
         <v>0.2</v>
@@ -7090,47 +7257,47 @@
     </row>
     <row r="35" spans="1:6" ht="15">
       <c r="A35" s="259" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D35" s="271">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="24" thickBot="1">
-      <c r="A36" s="300" t="s">
+      <c r="A36" s="303" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="300"/>
-      <c r="C36" s="300"/>
-      <c r="D36" s="300"/>
-      <c r="E36" s="300"/>
-      <c r="F36" s="300"/>
+      <c r="B36" s="303"/>
+      <c r="C36" s="303"/>
+      <c r="D36" s="303"/>
+      <c r="E36" s="303"/>
+      <c r="F36" s="303"/>
     </row>
     <row r="37" spans="1:6" ht="15">
       <c r="A37" s="244" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="301"/>
-      <c r="C37" s="301"/>
-      <c r="D37" s="301"/>
-      <c r="E37" s="301"/>
-      <c r="F37" s="302"/>
+      <c r="B37" s="304"/>
+      <c r="C37" s="304"/>
+      <c r="D37" s="304"/>
+      <c r="E37" s="304"/>
+      <c r="F37" s="305"/>
     </row>
     <row r="38" spans="1:6" ht="15">
       <c r="A38" s="245" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" s="246" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="246" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D38" s="246" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="246" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F38" s="247" t="s">
         <v>103</v>
@@ -7138,7 +7305,7 @@
     </row>
     <row r="39" spans="1:6" ht="15">
       <c r="A39" s="248" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B39" s="249"/>
       <c r="C39" s="249"/>
@@ -7153,7 +7320,7 @@
     </row>
     <row r="40" spans="1:6" ht="15">
       <c r="A40" s="248" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B40" s="249"/>
       <c r="C40" s="249"/>
@@ -7168,7 +7335,7 @@
     </row>
     <row r="41" spans="1:6" ht="15">
       <c r="A41" s="248" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B41" s="249"/>
       <c r="C41" s="249"/>
@@ -7183,7 +7350,7 @@
     </row>
     <row r="42" spans="1:6" ht="15">
       <c r="A42" s="248" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B42" s="249"/>
       <c r="C42" s="249"/>
@@ -7198,7 +7365,7 @@
     </row>
     <row r="43" spans="1:6" ht="15">
       <c r="A43" s="248" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B43" s="249"/>
       <c r="C43" s="249"/>
@@ -7213,7 +7380,7 @@
     </row>
     <row r="44" spans="1:6" ht="15">
       <c r="A44" s="248" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B44" s="249"/>
       <c r="C44" s="249"/>
@@ -7228,7 +7395,7 @@
     </row>
     <row r="45" spans="1:6" ht="15">
       <c r="A45" s="248" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B45" s="249"/>
       <c r="C45" s="249"/>
@@ -7243,7 +7410,7 @@
     </row>
     <row r="46" spans="1:6" ht="15">
       <c r="A46" s="248" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B46" s="249"/>
       <c r="C46" s="249"/>
@@ -7258,10 +7425,10 @@
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1">
       <c r="A47" s="250" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="303"/>
-      <c r="C47" s="304"/>
+        <v>128</v>
+      </c>
+      <c r="B47" s="306"/>
+      <c r="C47" s="307"/>
       <c r="D47" s="251">
         <f>SUM(D39:D46)</f>
         <v>100</v>
@@ -7274,7 +7441,7 @@
     </row>
     <row r="48" spans="1:6" ht="15">
       <c r="A48" s="263" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D48" s="261">
         <v>0.15</v>
@@ -7282,7 +7449,7 @@
     </row>
     <row r="49" spans="1:7" ht="15">
       <c r="A49" s="263" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D49" s="261">
         <v>0.2</v>
@@ -7290,10 +7457,10 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1">
       <c r="A50" s="272" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D50" s="271">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="24" thickBot="1">
@@ -7311,28 +7478,28 @@
       <c r="A52" s="237" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="291"/>
-      <c r="C52" s="292"/>
-      <c r="D52" s="292"/>
-      <c r="E52" s="292"/>
-      <c r="F52" s="293"/>
+      <c r="B52" s="294"/>
+      <c r="C52" s="295"/>
+      <c r="D52" s="295"/>
+      <c r="E52" s="295"/>
+      <c r="F52" s="296"/>
       <c r="G52" s="270"/>
     </row>
     <row r="53" spans="1:7" ht="15">
       <c r="A53" s="238" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B53" s="239" t="s">
         <v>48</v>
       </c>
       <c r="C53" s="239" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D53" s="239" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="239" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F53" s="240" t="s">
         <v>103</v>
@@ -7340,7 +7507,7 @@
     </row>
     <row r="54" spans="1:7" ht="15">
       <c r="A54" s="241" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B54" s="242"/>
       <c r="C54" s="242"/>
@@ -7355,7 +7522,7 @@
     </row>
     <row r="55" spans="1:7" ht="15">
       <c r="A55" s="241" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B55" s="242"/>
       <c r="C55" s="242"/>
@@ -7370,7 +7537,7 @@
     </row>
     <row r="56" spans="1:7" ht="15">
       <c r="A56" s="241" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B56" s="242"/>
       <c r="C56" s="242"/>
@@ -7385,7 +7552,7 @@
     </row>
     <row r="57" spans="1:7" ht="15">
       <c r="A57" s="241" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B57" s="242"/>
       <c r="C57" s="242"/>
@@ -7400,7 +7567,7 @@
     </row>
     <row r="58" spans="1:7" ht="15">
       <c r="A58" s="241" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B58" s="242"/>
       <c r="C58" s="242"/>
@@ -7415,7 +7582,7 @@
     </row>
     <row r="59" spans="1:7" ht="15">
       <c r="A59" s="241" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B59" s="242"/>
       <c r="C59" s="242"/>
@@ -7430,7 +7597,7 @@
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1">
       <c r="A60" s="253" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" s="254"/>
       <c r="C60" s="254"/>
@@ -7446,7 +7613,7 @@
     </row>
     <row r="61" spans="1:7" ht="15">
       <c r="A61" s="264" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="266">
         <v>0.15</v>
@@ -7454,7 +7621,7 @@
     </row>
     <row r="62" spans="1:7" ht="15">
       <c r="A62" s="264" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D62" s="266">
         <v>0.2</v>
@@ -7462,10 +7629,10 @@
     </row>
     <row r="63" spans="1:7" ht="15">
       <c r="A63" s="264" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D63" s="271">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -7504,8 +7671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C68761-F424-44AF-8353-006282F54B4A}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -7514,37 +7681,37 @@
     <col min="2" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A1" s="294" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="328"/>
+      <c r="A1" s="297" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="298"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="298"/>
+      <c r="E1" s="298"/>
+      <c r="F1" s="298"/>
+      <c r="G1" s="298"/>
+      <c r="H1" s="298"/>
+      <c r="I1" s="315"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A3" s="313" t="s">
+      <c r="A3" s="316" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="314"/>
-      <c r="C3" s="314"/>
-      <c r="D3" s="314"/>
-      <c r="E3" s="314"/>
-      <c r="F3" s="314"/>
-      <c r="G3" s="314"/>
-      <c r="H3" s="314"/>
-      <c r="I3" s="315"/>
+      <c r="B3" s="312"/>
+      <c r="C3" s="312"/>
+      <c r="D3" s="312"/>
+      <c r="E3" s="312"/>
+      <c r="F3" s="312"/>
+      <c r="G3" s="312"/>
+      <c r="H3" s="312"/>
+      <c r="I3" s="317"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" thickBot="1">
       <c r="A4" s="202"/>
@@ -7558,86 +7725,86 @@
       <c r="I4" s="203"/>
     </row>
     <row r="5" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A5" s="329" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="316" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="317"/>
-      <c r="D5" s="331" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="332"/>
-      <c r="F5" s="322" t="s">
+      <c r="A5" s="318" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="326" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="327"/>
+      <c r="D5" s="320" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="321"/>
+      <c r="F5" s="332" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="323"/>
-      <c r="H5" s="324" t="s">
+      <c r="G5" s="333"/>
+      <c r="H5" s="334" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="325"/>
-      <c r="J5" s="326" t="s">
+      <c r="I5" s="335"/>
+      <c r="J5" s="313" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="K5" s="314"/>
+      <c r="L5" s="314"/>
     </row>
     <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="330"/>
-      <c r="B6" s="281" t="s">
+      <c r="A6" s="319"/>
+      <c r="B6" s="282" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="205" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="280" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="286" t="s">
         <v>48</v>
       </c>
       <c r="E6" s="148" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="282" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="283" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="149" t="s">
-        <v>156</v>
-      </c>
-      <c r="H6" s="283" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="284" t="s">
         <v>48</v>
       </c>
       <c r="I6" s="150" t="s">
-        <v>156</v>
-      </c>
-      <c r="J6" s="279" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="279" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="279" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="285" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="285" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="279" t="s">
+      <c r="M6" s="285" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75">
-      <c r="A7" s="313" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="314"/>
-      <c r="C7" s="314"/>
-      <c r="D7" s="314"/>
-      <c r="E7" s="314"/>
-      <c r="F7" s="314"/>
-      <c r="G7" s="314"/>
-      <c r="H7" s="314"/>
-      <c r="I7" s="315"/>
+      <c r="A7" s="316" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="312"/>
+      <c r="C7" s="312"/>
+      <c r="D7" s="312"/>
+      <c r="E7" s="312"/>
+      <c r="F7" s="312"/>
+      <c r="G7" s="312"/>
+      <c r="H7" s="312"/>
+      <c r="I7" s="317"/>
     </row>
     <row r="8" spans="1:13" ht="60">
       <c r="A8" s="140" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B8" s="206">
         <v>0.5</v>
@@ -7645,7 +7812,9 @@
       <c r="C8" s="207">
         <v>9</v>
       </c>
-      <c r="D8" s="167"/>
+      <c r="D8" s="167">
+        <v>1</v>
+      </c>
       <c r="E8" s="151">
         <v>9</v>
       </c>
@@ -7658,20 +7827,25 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>159</v>
+        <v>170</v>
+      </c>
+      <c r="K8" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15">
       <c r="A9" s="141" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B9" s="208">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="209">
         <v>3</v>
       </c>
-      <c r="D9" s="168"/>
+      <c r="D9" s="168">
+        <v>0</v>
+      </c>
       <c r="E9" s="154">
         <v>3</v>
       </c>
@@ -7683,14 +7857,20 @@
       <c r="I9" s="156">
         <v>3</v>
       </c>
+      <c r="J9" t="s">
+        <v>173</v>
+      </c>
+      <c r="K9" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
       <c r="A10" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B10" s="211">
         <f>SUMPRODUCT(B8:B9,C8:C9)</f>
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="212">
         <f>SUM(C8:C9)</f>
@@ -7698,7 +7878,7 @@
       </c>
       <c r="D10" s="169">
         <f>SUMPRODUCT(D8:D9,E8:E9)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E10" s="160">
         <f>SUM(E8:E9)</f>
@@ -7720,26 +7900,23 @@
         <f>SUM(I8:I9)</f>
         <v>12</v>
       </c>
-      <c r="J10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="18.75">
-      <c r="A11" s="313" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="314"/>
-      <c r="C11" s="314"/>
-      <c r="D11" s="314"/>
-      <c r="E11" s="314"/>
-      <c r="F11" s="314"/>
-      <c r="G11" s="314"/>
-      <c r="H11" s="314"/>
-      <c r="I11" s="315"/>
+    </row>
+    <row r="11" spans="1:13" ht="19.5" thickBot="1">
+      <c r="A11" s="316" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="312"/>
+      <c r="C11" s="312"/>
+      <c r="D11" s="312"/>
+      <c r="E11" s="312"/>
+      <c r="F11" s="312"/>
+      <c r="G11" s="312"/>
+      <c r="H11" s="312"/>
+      <c r="I11" s="317"/>
     </row>
     <row r="12" spans="1:13" ht="30">
       <c r="A12" s="140" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B12" s="206">
         <v>1</v>
@@ -7747,7 +7924,9 @@
       <c r="C12" s="209">
         <v>9</v>
       </c>
-      <c r="D12" s="167"/>
+      <c r="D12" s="167">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="154">
         <v>9</v>
       </c>
@@ -7759,10 +7938,13 @@
       <c r="I12" s="153">
         <v>9</v>
       </c>
+      <c r="K12" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="30">
       <c r="A13" s="141" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B13" s="213">
         <v>1</v>
@@ -7770,7 +7952,9 @@
       <c r="C13" s="209">
         <v>2</v>
       </c>
-      <c r="D13" s="170"/>
+      <c r="D13" s="170">
+        <v>1</v>
+      </c>
       <c r="E13" s="154">
         <v>2</v>
       </c>
@@ -7785,7 +7969,7 @@
     </row>
     <row r="14" spans="1:13" ht="15">
       <c r="A14" s="142" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B14" s="214">
         <v>1</v>
@@ -7793,7 +7977,9 @@
       <c r="C14" s="209">
         <v>2</v>
       </c>
-      <c r="D14" s="171"/>
+      <c r="D14" s="171">
+        <v>1</v>
+      </c>
       <c r="E14" s="154">
         <v>2</v>
       </c>
@@ -7806,9 +7992,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1">
+    <row r="15" spans="1:13" ht="15">
       <c r="A15" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B15" s="211">
         <f>SUMPRODUCT(B12:B14,C12:C14)</f>
@@ -7820,7 +8006,7 @@
       </c>
       <c r="D15" s="169">
         <f>SUMPRODUCT(D12:D14,E12:E14)</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E15" s="157">
         <f>SUM(E12:E14)</f>
@@ -7844,21 +8030,25 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75">
-      <c r="A16" s="313" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="314"/>
-      <c r="C16" s="314"/>
-      <c r="D16" s="314"/>
-      <c r="E16" s="314"/>
-      <c r="F16" s="314"/>
-      <c r="G16" s="314"/>
-      <c r="H16" s="314"/>
-      <c r="I16" s="315"/>
-    </row>
-    <row r="17" spans="1:10" ht="15">
+      <c r="A16" s="281" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="312" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="312"/>
+      <c r="D16" s="312" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="312"/>
+      <c r="F16" s="278"/>
+      <c r="G16" s="278"/>
+      <c r="H16" s="278"/>
+      <c r="I16" s="279"/>
+    </row>
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="140" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B17" s="208">
         <v>1</v>
@@ -7866,7 +8056,9 @@
       <c r="C17" s="207">
         <v>2</v>
       </c>
-      <c r="D17" s="168"/>
+      <c r="D17" s="168">
+        <v>1</v>
+      </c>
       <c r="E17" s="151">
         <v>2</v>
       </c>
@@ -7879,9 +8071,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="141" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B18" s="208">
         <v>1</v>
@@ -7889,7 +8081,9 @@
       <c r="C18" s="209">
         <v>2</v>
       </c>
-      <c r="D18" s="168"/>
+      <c r="D18" s="168">
+        <v>1</v>
+      </c>
       <c r="E18" s="154">
         <v>2</v>
       </c>
@@ -7902,9 +8096,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="142" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B19" s="208">
         <v>1</v>
@@ -7912,7 +8106,9 @@
       <c r="C19" s="210">
         <v>2</v>
       </c>
-      <c r="D19" s="168"/>
+      <c r="D19" s="168">
+        <v>1</v>
+      </c>
       <c r="E19" s="157">
         <v>2</v>
       </c>
@@ -7925,9 +8121,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B20" s="211">
         <f>SUMPRODUCT(B17:B19,C17:C19)</f>
@@ -7939,7 +8135,7 @@
       </c>
       <c r="D20" s="169">
         <f>SUMPRODUCT(D17:D19,E17:E19)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E20" s="160">
         <f>SUM(E17:E19)</f>
@@ -7962,22 +8158,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="18.75">
-      <c r="A21" s="313" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="314"/>
-      <c r="C21" s="314"/>
-      <c r="D21" s="314"/>
-      <c r="E21" s="314"/>
-      <c r="F21" s="314"/>
-      <c r="G21" s="314"/>
-      <c r="H21" s="314"/>
-      <c r="I21" s="315"/>
-    </row>
-    <row r="22" spans="1:10" ht="30">
+    <row r="21" spans="1:11" ht="18.75">
+      <c r="A21" s="281" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="312" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="312"/>
+      <c r="D21" s="312" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="312"/>
+      <c r="F21" s="278"/>
+      <c r="G21" s="278"/>
+      <c r="H21" s="278"/>
+      <c r="I21" s="279"/>
+    </row>
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="141" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B22" s="213">
         <v>0.5</v>
@@ -7985,7 +8185,9 @@
       <c r="C22" s="209">
         <v>4</v>
       </c>
-      <c r="D22" s="170"/>
+      <c r="D22" s="170">
+        <v>1</v>
+      </c>
       <c r="E22" s="154">
         <v>4</v>
       </c>
@@ -7998,12 +8200,12 @@
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15">
       <c r="A23" s="142" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="B23" s="213">
         <v>1</v>
@@ -8011,7 +8213,9 @@
       <c r="C23" s="210">
         <v>4</v>
       </c>
-      <c r="D23" s="170"/>
+      <c r="D23" s="170">
+        <v>1</v>
+      </c>
       <c r="E23" s="157">
         <v>4</v>
       </c>
@@ -8024,9 +8228,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="90">
+    <row r="24" spans="1:11" ht="90">
       <c r="A24" s="142" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B24" s="213">
         <v>0</v>
@@ -8034,7 +8238,9 @@
       <c r="C24" s="210">
         <v>5</v>
       </c>
-      <c r="D24" s="170"/>
+      <c r="D24" s="170">
+        <v>1</v>
+      </c>
       <c r="E24" s="157">
         <v>5</v>
       </c>
@@ -8047,12 +8253,12 @@
         <v>5</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B25" s="211">
         <f>SUMPRODUCT(B22:B24,C22:C24)</f>
@@ -8064,7 +8270,7 @@
       </c>
       <c r="D25" s="169">
         <f>SUMPRODUCT(D22:D24,E22:E24)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E25" s="160">
         <f>SUM(E22:E24)</f>
@@ -8087,22 +8293,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18.75">
-      <c r="A26" s="313" t="s">
-        <v>177</v>
-      </c>
-      <c r="B26" s="314"/>
-      <c r="C26" s="314"/>
-      <c r="D26" s="314"/>
-      <c r="E26" s="314"/>
-      <c r="F26" s="314"/>
-      <c r="G26" s="314"/>
-      <c r="H26" s="314"/>
-      <c r="I26" s="315"/>
-    </row>
-    <row r="27" spans="1:10" ht="15">
+    <row r="26" spans="1:11" ht="18.75">
+      <c r="A26" s="281" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="312" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="312"/>
+      <c r="D26" s="312" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="312"/>
+      <c r="F26" s="278"/>
+      <c r="G26" s="278"/>
+      <c r="H26" s="278"/>
+      <c r="I26" s="279"/>
+    </row>
+    <row r="27" spans="1:11" ht="15">
       <c r="A27" s="140" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="B27" s="215">
         <v>1</v>
@@ -8110,7 +8320,9 @@
       <c r="C27" s="207">
         <v>2</v>
       </c>
-      <c r="D27" s="172"/>
+      <c r="D27" s="172">
+        <v>0.5</v>
+      </c>
       <c r="E27" s="151">
         <v>2</v>
       </c>
@@ -8122,10 +8334,13 @@
       <c r="I27" s="153">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15">
+      <c r="K27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15">
       <c r="A28" s="141" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B28" s="213">
         <v>1</v>
@@ -8133,7 +8348,9 @@
       <c r="C28" s="209">
         <v>3</v>
       </c>
-      <c r="D28" s="170"/>
+      <c r="D28" s="170">
+        <v>1</v>
+      </c>
       <c r="E28" s="154">
         <v>3</v>
       </c>
@@ -8146,9 +8363,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:11" ht="30">
       <c r="A29" s="142" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="B29" s="213">
         <v>1</v>
@@ -8156,7 +8373,9 @@
       <c r="C29" s="210">
         <v>3</v>
       </c>
-      <c r="D29" s="170"/>
+      <c r="D29" s="170">
+        <v>1</v>
+      </c>
       <c r="E29" s="157">
         <v>3</v>
       </c>
@@ -8169,9 +8388,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1">
       <c r="A30" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B30" s="216">
         <f>SUMPRODUCT(B27:B29,C27:C29)</f>
@@ -8183,7 +8402,7 @@
       </c>
       <c r="D30" s="145">
         <f>SUMPRODUCT(D27:D29,E27:E29)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E30" s="160">
         <f>SUM(E27:E29)</f>
@@ -8206,22 +8425,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="313" t="s">
-        <v>181</v>
-      </c>
-      <c r="B31" s="314"/>
-      <c r="C31" s="314"/>
-      <c r="D31" s="314"/>
-      <c r="E31" s="314"/>
-      <c r="F31" s="314"/>
-      <c r="G31" s="314"/>
-      <c r="H31" s="314"/>
-      <c r="I31" s="315"/>
-    </row>
-    <row r="32" spans="1:10" ht="15">
+    <row r="31" spans="1:11" ht="18.75">
+      <c r="A31" s="316" t="s">
+        <v>198</v>
+      </c>
+      <c r="B31" s="312"/>
+      <c r="C31" s="312"/>
+      <c r="D31" s="312"/>
+      <c r="E31" s="312"/>
+      <c r="F31" s="312"/>
+      <c r="G31" s="312"/>
+      <c r="H31" s="312"/>
+      <c r="I31" s="317"/>
+    </row>
+    <row r="32" spans="1:11" ht="15">
       <c r="A32" s="141" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="B32" s="213">
         <v>1</v>
@@ -8229,7 +8448,9 @@
       <c r="C32" s="209">
         <v>3</v>
       </c>
-      <c r="D32" s="170"/>
+      <c r="D32" s="170">
+        <v>1</v>
+      </c>
       <c r="E32" s="154">
         <v>3</v>
       </c>
@@ -8242,9 +8463,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30">
+    <row r="33" spans="1:11" ht="30">
       <c r="A33" s="141" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="B33" s="213">
         <v>1</v>
@@ -8252,7 +8473,9 @@
       <c r="C33" s="209">
         <v>4</v>
       </c>
-      <c r="D33" s="170"/>
+      <c r="D33" s="170">
+        <v>1</v>
+      </c>
       <c r="E33" s="154">
         <v>4</v>
       </c>
@@ -8265,9 +8488,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30">
+    <row r="34" spans="1:11" ht="30">
       <c r="A34" s="141" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B34" s="213">
         <v>1</v>
@@ -8275,7 +8498,9 @@
       <c r="C34" s="209">
         <v>3</v>
       </c>
-      <c r="D34" s="170"/>
+      <c r="D34" s="170">
+        <v>1</v>
+      </c>
       <c r="E34" s="154">
         <v>3</v>
       </c>
@@ -8288,9 +8513,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15">
+    <row r="35" spans="1:11" ht="15">
       <c r="A35" s="141" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="B35" s="213">
         <v>1</v>
@@ -8298,7 +8523,9 @@
       <c r="C35" s="209">
         <v>4</v>
       </c>
-      <c r="D35" s="170"/>
+      <c r="D35" s="170">
+        <v>1</v>
+      </c>
       <c r="E35" s="154">
         <v>4</v>
       </c>
@@ -8311,9 +8538,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15">
+    <row r="36" spans="1:11" ht="15">
       <c r="A36" s="141" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="B36" s="213">
         <v>0.5</v>
@@ -8321,7 +8548,9 @@
       <c r="C36" s="209">
         <v>4</v>
       </c>
-      <c r="D36" s="170"/>
+      <c r="D36" s="170">
+        <v>1</v>
+      </c>
       <c r="E36" s="154">
         <v>4</v>
       </c>
@@ -8334,12 +8563,12 @@
         <v>4</v>
       </c>
       <c r="J36" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15">
       <c r="A37" s="141" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="B37" s="213">
         <v>1</v>
@@ -8347,7 +8576,9 @@
       <c r="C37" s="209">
         <v>2</v>
       </c>
-      <c r="D37" s="170"/>
+      <c r="D37" s="170">
+        <v>1</v>
+      </c>
       <c r="E37" s="154">
         <v>2</v>
       </c>
@@ -8360,9 +8591,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:11" ht="30">
       <c r="A38" s="142" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B38" s="213">
         <v>1</v>
@@ -8370,7 +8601,9 @@
       <c r="C38" s="210">
         <v>10</v>
       </c>
-      <c r="D38" s="170"/>
+      <c r="D38" s="170">
+        <v>1</v>
+      </c>
       <c r="E38" s="157">
         <v>10</v>
       </c>
@@ -8383,9 +8616,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15">
+    <row r="39" spans="1:11" ht="15">
       <c r="A39" s="142" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="B39" s="213">
         <v>1</v>
@@ -8393,7 +8626,9 @@
       <c r="C39" s="210">
         <v>4</v>
       </c>
-      <c r="D39" s="170"/>
+      <c r="D39" s="170">
+        <v>1</v>
+      </c>
       <c r="E39" s="157">
         <v>4</v>
       </c>
@@ -8406,9 +8641,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15">
+    <row r="40" spans="1:11" ht="15">
       <c r="A40" s="142" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="B40" s="213">
         <v>1</v>
@@ -8416,7 +8651,9 @@
       <c r="C40" s="210">
         <v>3</v>
       </c>
-      <c r="D40" s="170"/>
+      <c r="D40" s="170">
+        <v>1</v>
+      </c>
       <c r="E40" s="157">
         <v>3</v>
       </c>
@@ -8429,9 +8666,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1">
       <c r="A41" s="146" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B41" s="216">
         <f>SUMPRODUCT(B32:B40,C32:C40)</f>
@@ -8443,7 +8680,7 @@
       </c>
       <c r="D41" s="145">
         <f>SUMPRODUCT(D32:D40,E32:E40)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E41" s="160">
         <f>SUM(E32:E40)</f>
@@ -8466,22 +8703,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="18.75">
-      <c r="A42" s="313" t="s">
-        <v>192</v>
-      </c>
-      <c r="B42" s="314"/>
-      <c r="C42" s="314"/>
-      <c r="D42" s="314"/>
-      <c r="E42" s="314"/>
-      <c r="F42" s="314"/>
-      <c r="G42" s="314"/>
-      <c r="H42" s="314"/>
-      <c r="I42" s="315"/>
-    </row>
-    <row r="43" spans="1:10" ht="30">
+    <row r="42" spans="1:11" ht="18.75">
+      <c r="A42" s="316" t="s">
+        <v>209</v>
+      </c>
+      <c r="B42" s="312"/>
+      <c r="C42" s="312"/>
+      <c r="D42" s="312"/>
+      <c r="E42" s="312"/>
+      <c r="F42" s="312"/>
+      <c r="G42" s="312"/>
+      <c r="H42" s="312"/>
+      <c r="I42" s="317"/>
+    </row>
+    <row r="43" spans="1:11" ht="30">
       <c r="A43" s="144" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B43" s="215">
         <v>1</v>
@@ -8489,7 +8726,9 @@
       <c r="C43" s="217">
         <v>3</v>
       </c>
-      <c r="D43" s="172"/>
+      <c r="D43" s="172">
+        <v>1</v>
+      </c>
       <c r="E43" s="161">
         <v>3</v>
       </c>
@@ -8502,9 +8741,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:11" ht="30">
       <c r="A44" s="142" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B44" s="213">
         <v>1</v>
@@ -8512,7 +8751,9 @@
       <c r="C44" s="210">
         <v>4</v>
       </c>
-      <c r="D44" s="170"/>
+      <c r="D44" s="170">
+        <v>1</v>
+      </c>
       <c r="E44" s="157">
         <v>4</v>
       </c>
@@ -8525,9 +8766,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="45">
+    <row r="45" spans="1:11" ht="45">
       <c r="A45" s="143" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="B45" s="213">
         <v>1</v>
@@ -8535,7 +8776,9 @@
       <c r="C45" s="209">
         <v>4</v>
       </c>
-      <c r="D45" s="170"/>
+      <c r="D45" s="170">
+        <v>0.5</v>
+      </c>
       <c r="E45" s="154">
         <v>4</v>
       </c>
@@ -8547,10 +8790,13 @@
       <c r="I45" s="159">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1">
+      <c r="K45" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1">
       <c r="A46" s="147" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B46" s="211">
         <f>SUMPRODUCT(B43:B45,C43:C45)</f>
@@ -8562,7 +8808,7 @@
       </c>
       <c r="D46" s="169">
         <f>SUMPRODUCT(D43:D45,E43:E45)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E46" s="160">
         <f>SUM(E43:E45)</f>
@@ -8585,91 +8831,85 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A47" s="313" t="s">
+    <row r="47" spans="1:11" ht="19.5" thickBot="1">
+      <c r="A47" s="316" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="314"/>
-      <c r="C47" s="314"/>
-      <c r="D47" s="314"/>
-      <c r="E47" s="314"/>
-      <c r="F47" s="314"/>
-      <c r="G47" s="314"/>
-      <c r="H47" s="314"/>
-      <c r="I47" s="315"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1">
+      <c r="B47" s="312"/>
+      <c r="C47" s="312"/>
+      <c r="D47" s="312"/>
+      <c r="E47" s="312"/>
+      <c r="F47" s="312"/>
+      <c r="G47" s="312"/>
+      <c r="H47" s="312"/>
+      <c r="I47" s="317"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1">
       <c r="A48" s="187" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="B48" s="218">
-        <f>B10+B15+B20+B25+B30+B41+B46</f>
-        <v>86.5</v>
+        <f t="shared" ref="B48:I48" si="0">B10+B15+B20+B25+B30+B41+B46</f>
+        <v>85</v>
       </c>
       <c r="C48" s="219">
-        <f>C10+C15+C20+C25+C30+C41+C46</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D48" s="173">
-        <f>D10+D15+D20+D25+D30+D41+D46</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>89.5</v>
       </c>
       <c r="E48" s="164">
-        <f>E10+E15+E20+E25+E30+E41+E46</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F48" s="180">
-        <f>F10+F15+F20+F25+F30+F41+F46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G48" s="165">
-        <f>G10+G15+G20+G25+G30+G41+G46</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="H48" s="186">
-        <f>H10+H15+H20+H25+H30+H41+H46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I48" s="166">
-        <f>I10+I15+I20+I25+I30+I41+I46</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="187" t="s">
-        <v>197</v>
-      </c>
-      <c r="B49" s="318">
+        <v>215</v>
+      </c>
+      <c r="B49" s="328">
         <f>B48/C48</f>
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="C49" s="319"/>
-      <c r="D49" s="320">
+        <v>0.85</v>
+      </c>
+      <c r="C49" s="329"/>
+      <c r="D49" s="330">
         <f>D48/E48</f>
-        <v>0</v>
-      </c>
-      <c r="E49" s="321"/>
-      <c r="F49" s="309">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E49" s="331"/>
+      <c r="F49" s="322">
         <f>F48/G48</f>
         <v>0</v>
       </c>
-      <c r="G49" s="310"/>
-      <c r="H49" s="311">
+      <c r="G49" s="323"/>
+      <c r="H49" s="324">
         <f>H48/I48</f>
         <v>0</v>
       </c>
-      <c r="I49" s="312"/>
+      <c r="I49" s="325"/>
     </row>
     <row r="50" spans="1:9" ht="15"/>
     <row r="51" spans="1:9" ht="15"/>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:E5"/>
+  <mergeCells count="23">
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="H49:I49"/>
     <mergeCell ref="A42:I42"/>
@@ -8680,10 +8920,19 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="A47:I47"/>
     <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A16:I16"/>
     <mergeCell ref="A11:I11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H41 H10 H25 H15 H20 H30" xr:uid="{4EF0FB88-23AB-454B-A6DC-A652F4C1E260}">
@@ -8701,15 +8950,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B41E0342602C49449CD93109DBCAB8C5" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cab946e3812a26735e8b0dc00d59aca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3ea4e87-b30d-4ccc-9564-7710f23c54f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afa808ced5dc9827eedaaa69eb8b35dd" ns2:_="">
     <xsd:import namespace="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
@@ -8841,6 +9081,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8848,11 +9097,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59738D7-B2D0-4EAF-BA9A-9311EB45CEF2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA4AA86D-FB09-42E5-A9C7-0D47AFD487FC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA4AA86D-FB09-42E5-A9C7-0D47AFD487FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59738D7-B2D0-4EAF-BA9A-9311EB45CEF2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>